<commit_message>
Desglose y creacion de Testcases variados
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/DataSet.xlsx
+++ b/src/test/resources/Data/DataSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IntegradorS5\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A644E94-CA2B-47A4-90E0-30FF499F2C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C6A9DF-DBE9-4A78-8307-9D02FC6F587F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{AC655BA4-9BA8-473A-B22E-609358072BB5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>CasosDePrueba</t>
   </si>
@@ -115,13 +115,22 @@
   </si>
   <si>
     <t>16-9-2005</t>
+  </si>
+  <si>
+    <t>CP004</t>
+  </si>
+  <si>
+    <t>CP005</t>
+  </si>
+  <si>
+    <t>16-9-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,14 +140,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,26 +169,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,10 +534,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD430A2E-A63F-405C-B109-AA7701175DE0}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -601,62 +599,155 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3">
-        <v>66565423</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="3">
-        <v>1123456789</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="3">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2">
+        <v>66565424</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1123456789</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="26" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2">
+        <v>66565424</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1123456789</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="26" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>66565426</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1123456789</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="2">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>